<commit_message>
revised data based on research feedback
</commit_message>
<xml_diff>
--- a/data/sankey_data.xlsx
+++ b/data/sankey_data.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21500" yWindow="2800" windowWidth="22160" windowHeight="17060"/>
+    <workbookView xWindow="29040" yWindow="460" windowWidth="22160" windowHeight="17060"/>
   </bookViews>
   <sheets>
     <sheet name="Sankey data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -107,21 +107,6 @@
     <t>Other Bach</t>
   </si>
   <si>
-    <t>White Teaching degree</t>
-  </si>
-  <si>
-    <t>Hispanic Teaching degree</t>
-  </si>
-  <si>
-    <t>Black Teaching degree</t>
-  </si>
-  <si>
-    <t>Asian Teaching degree</t>
-  </si>
-  <si>
-    <t>Other Teaching degree</t>
-  </si>
-  <si>
     <t>Black Teacher-degree</t>
   </si>
   <si>
@@ -189,6 +174,21 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>White-Teaching degree</t>
+  </si>
+  <si>
+    <t>Black-Teaching degree</t>
+  </si>
+  <si>
+    <t>Hispanic-Teaching degree</t>
+  </si>
+  <si>
+    <t>Asian-Teaching degree</t>
+  </si>
+  <si>
+    <t>Other-Teaching degree</t>
   </si>
 </sst>
 </file>
@@ -241,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -256,6 +256,8 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -574,17 +576,17 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="11.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.796875" customWidth="1"/>
-    <col min="9" max="9" width="16.796875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -607,10 +609,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -639,6 +641,9 @@
         <f>SUM(F2:F7)</f>
         <v>24810849</v>
       </c>
+      <c r="K2" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -666,6 +671,9 @@
         <f>SUM(F8:F13)</f>
         <v>6124591</v>
       </c>
+      <c r="K3" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -693,6 +701,9 @@
         <f>SUM(F14:F19)</f>
         <v>8861370</v>
       </c>
+      <c r="K4" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -720,6 +731,9 @@
         <f>SUM(F20:F25)</f>
         <v>3393171</v>
       </c>
+      <c r="K5" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -747,8 +761,11 @@
         <f>SUM(F26:F31)</f>
         <v>634487</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="K6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -774,6 +791,10 @@
         <f>SUM(F3:F7)</f>
         <v>23408059</v>
       </c>
+      <c r="K7">
+        <f>J7/J2</f>
+        <v>0.94346062079536253</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -801,9 +822,13 @@
         <f>SUM(F9:F13)</f>
         <v>5453028</v>
       </c>
+      <c r="K8">
+        <f>J8/J3</f>
+        <v>0.8903497392723857</v>
+      </c>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -829,6 +854,10 @@
         <f>SUM(F15:F19)</f>
         <v>6659753</v>
       </c>
+      <c r="K9">
+        <f>J9/J4</f>
+        <v>0.7515489139941115</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -856,8 +885,12 @@
         <f>SUM(F21:F25)</f>
         <v>3227421</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <f>J10/J5</f>
+        <v>0.95115188712858856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -883,6 +916,10 @@
         <f>SUM(F27:F31)</f>
         <v>556792</v>
       </c>
+      <c r="K11">
+        <f>J11/J6</f>
+        <v>0.8775467424864497</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -910,6 +947,10 @@
         <f>SUM(F4:F7)</f>
         <v>10010319</v>
       </c>
+      <c r="K12" s="11">
+        <f>J12/J7</f>
+        <v>0.42764412888740583</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -937,6 +978,10 @@
         <f>SUM(F10:F13)</f>
         <v>1315379</v>
       </c>
+      <c r="K13" s="11">
+        <f>J13/J8</f>
+        <v>0.24121992404953724</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -964,6 +1009,10 @@
         <f>SUM(F16:F19)</f>
         <v>1431034</v>
       </c>
+      <c r="K14" s="11">
+        <f>J14/J9</f>
+        <v>0.21487793916681294</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -991,6 +1040,10 @@
         <f>SUM(F22:F25)</f>
         <v>2097650</v>
       </c>
+      <c r="K15" s="11">
+        <f>J15/J10</f>
+        <v>0.64994619542972543</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1018,8 +1071,12 @@
         <f>SUM(F28:F31)</f>
         <v>146214</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K16" s="11">
+        <f>J16/J6</f>
+        <v>0.23044443778989956</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1039,14 +1096,18 @@
         <v>77780</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="J17" s="2">
         <f>SUM(F6:F7)</f>
         <v>913874</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K17" s="11">
+        <f>J17/J12</f>
+        <v>9.1293194552541229E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1066,14 +1127,18 @@
         <v>45373</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="J18" s="2">
         <f>SUM(F12:F13)</f>
         <v>83039</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K18" s="11">
+        <f>J18/J13</f>
+        <v>6.312933382698066E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1093,14 +1158,18 @@
         <v>56613</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="J19" s="2">
         <f>SUM(F18:F19)</f>
         <v>101986</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K19" s="11">
+        <f>J19/J14</f>
+        <v>7.1267349343202183E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1120,14 +1189,18 @@
         <v>165750</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="J20" s="2">
         <f>SUM(F24:F25)</f>
         <v>52831</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K20" s="11">
+        <f>J20/J15</f>
+        <v>2.5185803160679809E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1147,14 +1220,18 @@
         <v>1129771</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="J21" s="2">
         <f>SUM(F30:F31)</f>
         <v>12002</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K21" s="11">
+        <f>J21/J16</f>
+        <v>8.2085162843503354E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1174,14 +1251,18 @@
         <v>1987973</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="J22" s="2">
         <f>F7</f>
         <v>575757</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K22" s="11">
+        <f>J22/J17</f>
+        <v>0.63001792369626453</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1201,14 +1282,18 @@
         <v>56846</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J23" s="2">
         <f>F13</f>
         <v>43283</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K23" s="11">
+        <f>J23/J18</f>
+        <v>0.52123700911619841</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1228,14 +1313,18 @@
         <v>33132</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J24" s="2">
         <f>F19</f>
         <v>56613</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K24" s="11">
+        <f>J24/J19</f>
+        <v>0.55510560272978648</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1255,14 +1344,18 @@
         <v>19699</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J25" s="2">
         <f>F25</f>
         <v>19699</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K25" s="11">
+        <f>J25/J20</f>
+        <v>0.37286820238117774</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1282,14 +1375,18 @@
         <v>77695</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J26" s="2">
         <f>F31</f>
         <v>5853</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K26" s="11">
+        <f>J26/J21</f>
+        <v>0.48766872187968674</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1309,14 +1406,18 @@
         <v>410578</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J27" s="2">
         <f>F5</f>
         <v>505537</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K27" s="11">
+        <f>J27/J12</f>
+        <v>5.0501587411949607E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1336,14 +1437,18 @@
         <v>127276</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J28" s="2">
         <f>F11</f>
         <v>69675</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K28" s="11">
+        <f>J28/J13</f>
+        <v>5.2969524372823346E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1363,14 +1468,18 @@
         <v>6936</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J29" s="2">
         <f>F17</f>
         <v>77780</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K29" s="11">
+        <f>J29/J14</f>
+        <v>5.4352307492344695E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1390,14 +1499,18 @@
         <v>6149</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J30" s="2">
         <f>F23</f>
         <v>56846</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K30" s="11">
+        <f>J30/J15</f>
+        <v>2.7099849831954806E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -1417,111 +1530,126 @@
         <v>5853</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J31" s="2">
         <f>F29</f>
         <v>6936</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K31" s="11">
+        <f>J31/J16</f>
+        <v>4.7437317903894292E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="I32" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J32" s="2">
         <f>SUM(J22,J27)</f>
         <v>1081294</v>
       </c>
-    </row>
-    <row r="33" spans="9:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K32" s="11"/>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I33" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J33" s="2">
         <f>SUM(J23,J28)</f>
         <v>112958</v>
       </c>
-    </row>
-    <row r="34" spans="9:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K33" s="11"/>
+    </row>
+    <row r="34" spans="9:11" ht="30" x14ac:dyDescent="0.2">
       <c r="I34" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J34" s="2">
         <f>SUM(J24,J29)</f>
         <v>134393</v>
       </c>
-    </row>
-    <row r="35" spans="9:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K34" s="11"/>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I35" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J35" s="2">
         <f>SUM(J25,J30)</f>
         <v>76545</v>
       </c>
-    </row>
-    <row r="36" spans="9:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K35" s="11"/>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I36" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J36" s="2">
         <f>SUM(J26,J31)</f>
         <v>12789</v>
       </c>
-    </row>
-    <row r="37" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="11"/>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I37" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J37" s="2">
         <f>SUM(J32:J36)</f>
         <v>1417979</v>
       </c>
-    </row>
-    <row r="38" spans="9:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K37" s="11"/>
+    </row>
+    <row r="38" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I38" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J38" s="2">
         <f>J37-J32</f>
         <v>336685</v>
       </c>
-    </row>
-    <row r="39" spans="9:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K38" s="11"/>
+    </row>
+    <row r="39" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I39" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J39" s="2">
         <f>J37-J33</f>
         <v>1305021</v>
       </c>
-    </row>
-    <row r="40" spans="9:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K39" s="11"/>
+    </row>
+    <row r="40" spans="9:11" ht="30" x14ac:dyDescent="0.2">
       <c r="I40" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J40" s="2">
         <f>J37-J34</f>
         <v>1283586</v>
       </c>
-    </row>
-    <row r="41" spans="9:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K40" s="11"/>
+    </row>
+    <row r="41" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I41" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J41" s="2">
         <f>J37-J35</f>
         <v>1341434</v>
       </c>
-    </row>
-    <row r="42" spans="9:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="K41" s="11"/>
+    </row>
+    <row r="42" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I42" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J42" s="2">
         <f>J37-J36</f>
         <v>1405190</v>
       </c>
+      <c r="K42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revised data and added side labels
</commit_message>
<xml_diff>
--- a/data/sankey_data.xlsx
+++ b/data/sankey_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivhou/Documents/Urban/teacher-diversity/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhou/Documents/Projects/teacher-diversity/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10320" yWindow="1040" windowWidth="22160" windowHeight="17060"/>
+    <workbookView xWindow="25940" yWindow="9300" windowWidth="22160" windowHeight="17060"/>
   </bookViews>
   <sheets>
     <sheet name="Sankey data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>wbhao</t>
   </si>
@@ -173,6 +173,9 @@
     <t>Category</t>
   </si>
   <si>
+    <t>Value</t>
+  </si>
+  <si>
     <t>White-Teaching degree</t>
   </si>
   <si>
@@ -188,19 +191,26 @@
     <t>Other-Teaching degree</t>
   </si>
   <si>
-    <t>Actual value</t>
-  </si>
-  <si>
-    <t>Relative value</t>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Relative Percent</t>
+  </si>
+  <si>
+    <t>Bachelors</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -244,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -259,10 +269,9 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -578,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -592,10 +601,10 @@
     <col min="7" max="7" width="17.83203125" customWidth="1"/>
     <col min="9" max="9" width="16.83203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -618,13 +627,22 @@
         <v>47</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -650,14 +668,17 @@
         <f>SUM(F2:F7)</f>
         <v>24810849</v>
       </c>
-      <c r="K2" s="10">
-        <v>1</v>
-      </c>
-      <c r="L2" s="12">
+      <c r="K2" s="12">
+        <v>1</v>
+      </c>
+      <c r="L2">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -683,14 +704,17 @@
         <f>SUM(F8:F13)</f>
         <v>6124591</v>
       </c>
-      <c r="K3" s="10">
-        <v>1</v>
-      </c>
-      <c r="L3" s="12">
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -716,14 +740,17 @@
         <f>SUM(F14:F19)</f>
         <v>8861370</v>
       </c>
-      <c r="K4" s="10">
-        <v>1</v>
-      </c>
-      <c r="L4" s="12">
+      <c r="K4" s="12">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -749,14 +776,17 @@
         <f>SUM(F20:F25)</f>
         <v>3393171</v>
       </c>
-      <c r="K5" s="10">
-        <v>1</v>
-      </c>
-      <c r="L5" s="12">
+      <c r="K5" s="12">
+        <v>1</v>
+      </c>
+      <c r="L5">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N5" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -782,14 +812,17 @@
         <f>SUM(F26:F31)</f>
         <v>634487</v>
       </c>
-      <c r="K6" s="10">
-        <v>1</v>
-      </c>
-      <c r="L6" s="12">
+      <c r="K6" s="12">
+        <v>1</v>
+      </c>
+      <c r="L6">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N6" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -815,16 +848,20 @@
         <f>SUM(F3:F7)</f>
         <v>23408059</v>
       </c>
-      <c r="K7">
-        <f t="shared" ref="K7:K15" si="0">J7/J2</f>
+      <c r="K7" s="12">
+        <f>J7/J2</f>
         <v>0.94346062079536253</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7">
         <f>K7*L2</f>
         <v>943460.62079536251</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N7">
+        <f>J7/J2</f>
+        <v>0.94346062079536253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -850,16 +887,20 @@
         <f>SUM(F9:F13)</f>
         <v>5453028</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
+      <c r="K8" s="12">
+        <f>J8/J3</f>
         <v>0.8903497392723857</v>
       </c>
-      <c r="L8" s="12">
-        <f>K8*L3</f>
+      <c r="L8" s="2">
+        <f>K8*L2</f>
         <v>890349.73927238572</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N8">
+        <f>J8/J3</f>
+        <v>0.8903497392723857</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -885,16 +926,20 @@
         <f>SUM(F15:F19)</f>
         <v>6659753</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
+      <c r="K9" s="12">
+        <f>J9/J4</f>
         <v>0.7515489139941115</v>
       </c>
-      <c r="L9" s="12">
-        <f>K9*L4</f>
+      <c r="L9">
+        <f t="shared" ref="L9" si="0">K9*L4</f>
         <v>751548.91399411147</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N9">
+        <f>J9/J4</f>
+        <v>0.7515489139941115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -920,16 +965,20 @@
         <f>SUM(F21:F25)</f>
         <v>3227421</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
+      <c r="K10" s="12">
+        <f>J10/J5</f>
         <v>0.95115188712858856</v>
       </c>
-      <c r="L10" s="12">
-        <f>K10*L5</f>
+      <c r="L10" s="2">
+        <f t="shared" ref="L10" si="1">K10*L4</f>
         <v>951151.88712858851</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <f>J10/J5</f>
+        <v>0.95115188712858856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -955,16 +1004,20 @@
         <f>SUM(F27:F31)</f>
         <v>556792</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
+      <c r="K11" s="12">
+        <f>J11/J6</f>
         <v>0.8775467424864497</v>
       </c>
-      <c r="L11" s="12">
-        <f>K11*L6</f>
+      <c r="L11">
+        <f t="shared" ref="L11" si="2">K11*L6</f>
         <v>877546.74248644966</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <f>J11/J6</f>
+        <v>0.8775467424864497</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -990,16 +1043,23 @@
         <f>SUM(F4:F7)</f>
         <v>10010319</v>
       </c>
-      <c r="K12" s="11">
-        <f t="shared" si="0"/>
+      <c r="K12" s="12">
+        <f>J12/J7</f>
         <v>0.42764412888740583</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12">
         <f>K12*L7</f>
         <v>403465.39531960391</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <f>J12/J2</f>
+        <v>0.40346539531960396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1025,16 +1085,23 @@
         <f>SUM(F10:F13)</f>
         <v>1315379</v>
       </c>
-      <c r="K13" s="11">
-        <f t="shared" si="0"/>
+      <c r="K13" s="12">
+        <f>J13/J8</f>
         <v>0.24121992404953724</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13">
         <f>K13*L8</f>
         <v>214770.09648481017</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f>J13/J3</f>
+        <v>0.21477009648481016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1060,16 +1127,23 @@
         <f>SUM(F16:F19)</f>
         <v>1431034</v>
       </c>
-      <c r="K14" s="11">
-        <f t="shared" si="0"/>
+      <c r="K14" s="12">
+        <f>J14/J9</f>
         <v>0.21487793916681294</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14">
         <f>K14*L9</f>
         <v>161491.28182211102</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <f>J14/J4</f>
+        <v>0.16149128182211103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1095,16 +1169,23 @@
         <f>SUM(F22:F25)</f>
         <v>2097650</v>
       </c>
-      <c r="K15" s="11">
-        <f t="shared" si="0"/>
+      <c r="K15" s="12">
+        <f>J15/J10</f>
         <v>0.64994619542972543</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15">
         <f>K15*L10</f>
         <v>618197.55031502969</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <f>J15/J5</f>
+        <v>0.61819755031502976</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1130,16 +1211,23 @@
         <f>SUM(F28:F31)</f>
         <v>146214</v>
       </c>
-      <c r="K16" s="11">
-        <f>J16/J11</f>
-        <v>0.26260075575798503</v>
-      </c>
-      <c r="L16" s="12">
+      <c r="K16" s="12">
+        <f>J16/J6</f>
+        <v>0.23044443778989956</v>
+      </c>
+      <c r="L16">
         <f>K16*L11</f>
-        <v>230444.43778989956</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+        <v>202225.76570664765</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <f>J16/J6</f>
+        <v>0.23044443778989956</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1159,22 +1247,30 @@
         <v>77780</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J17" s="2">
         <f>SUM(F6:F7)</f>
         <v>913874</v>
       </c>
-      <c r="K17" s="11">
-        <f t="shared" ref="K17:K26" si="1">J17/J12</f>
+      <c r="K17" s="12">
+        <f>J17/J12</f>
         <v>9.1293194552541229E-2</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17">
         <f>K17*L12</f>
         <v>36833.644830130557</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <f>J17/J12</f>
+        <v>9.1293194552541229E-2</v>
+      </c>
+      <c r="N17">
+        <f>J17/J2</f>
+        <v>3.683364483013056E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1194,22 +1290,30 @@
         <v>45373</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J18" s="2">
         <f>SUM(F12:F13)</f>
         <v>83039</v>
       </c>
-      <c r="K18" s="11">
-        <f t="shared" si="1"/>
+      <c r="K18" s="12">
+        <f>J18/J13</f>
         <v>6.312933382698066E-2</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18">
         <f>K18*L13</f>
         <v>13558.293117042427</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <f>J18/J13</f>
+        <v>6.312933382698066E-2</v>
+      </c>
+      <c r="N18">
+        <f>J18/J3</f>
+        <v>1.3558293117042429E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1229,22 +1333,30 @@
         <v>56613</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J19" s="2">
         <f>SUM(F18:F19)</f>
         <v>101986</v>
       </c>
-      <c r="K19" s="11">
-        <f t="shared" si="1"/>
+      <c r="K19" s="12">
+        <f>J19/J14</f>
         <v>7.1267349343202183E-2</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19">
         <f>K19*L14</f>
         <v>11509.055597497902</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <f>J19/J14</f>
+        <v>7.1267349343202183E-2</v>
+      </c>
+      <c r="N19">
+        <f>J19/J4</f>
+        <v>1.1509055597497904E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1264,22 +1376,30 @@
         <v>165750</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J20" s="2">
         <f>SUM(F24:F25)</f>
         <v>52831</v>
       </c>
-      <c r="K20" s="11">
-        <f t="shared" si="1"/>
+      <c r="K20" s="12">
+        <f>J20/J15</f>
         <v>2.5185803160679809E-2</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20">
         <f>K20*L15</f>
         <v>15569.801816648791</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <f>J20/J15</f>
+        <v>2.5185803160679809E-2</v>
+      </c>
+      <c r="N20">
+        <f>J20/J5</f>
+        <v>1.5569801816648793E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1299,22 +1419,30 @@
         <v>1129771</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J21" s="2">
         <f>SUM(F30:F31)</f>
         <v>12002</v>
       </c>
-      <c r="K21" s="11">
-        <f t="shared" si="1"/>
+      <c r="K21" s="12">
+        <f>J21/J16</f>
         <v>8.2085162843503354E-2</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21">
         <f>K21*L16</f>
-        <v>18916.069202363484</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+        <v>16599.734909182327</v>
+      </c>
+      <c r="M21">
+        <f>J21/J16</f>
+        <v>8.2085162843503354E-2</v>
+      </c>
+      <c r="N21">
+        <f>J21/J6</f>
+        <v>1.8916069202363484E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1340,16 +1468,24 @@
         <f>F7</f>
         <v>575757</v>
       </c>
-      <c r="K22" s="11">
-        <f t="shared" si="1"/>
+      <c r="K22" s="12">
+        <f>J22/J17</f>
         <v>0.63001792369626453</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22">
         <f>K22*L17</f>
         <v>23205.856438044502</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <f>J22/J12</f>
+        <v>5.7516348879591152E-2</v>
+      </c>
+      <c r="N22">
+        <f>J22/J2</f>
+        <v>2.3205856438044504E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1375,16 +1511,24 @@
         <f>F13</f>
         <v>43283</v>
       </c>
-      <c r="K23" s="11">
-        <f t="shared" si="1"/>
+      <c r="K23" s="12">
+        <f>J23/J18</f>
         <v>0.52123700911619841</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23">
         <f>K23*L18</f>
         <v>7067.0841530479338</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <f>J23/J13</f>
+        <v>3.2905345151473454E-2</v>
+      </c>
+      <c r="N23">
+        <f>J23/J3</f>
+        <v>7.0670841530479341E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1410,16 +1554,24 @@
         <f>F19</f>
         <v>56613</v>
       </c>
-      <c r="K24" s="11">
-        <f t="shared" si="1"/>
+      <c r="K24" s="12">
+        <f>J24/J19</f>
         <v>0.55510560272978648</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24">
         <f>K24*L19</f>
         <v>6388.7412442996956</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <f>J24/J14</f>
+        <v>3.9560904912112498E-2</v>
+      </c>
+      <c r="N24">
+        <f>J24/J4</f>
+        <v>6.3887412442996967E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1445,16 +1597,24 @@
         <f>F25</f>
         <v>19699</v>
       </c>
-      <c r="K25" s="11">
-        <f t="shared" si="1"/>
+      <c r="K25" s="12">
+        <f>J25/J20</f>
         <v>0.37286820238117774</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25">
         <f>K25*L20</f>
         <v>5805.4840148050298</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <f>J25/J15</f>
+        <v>9.390985150048865E-3</v>
+      </c>
+      <c r="N25">
+        <f>J25/J5</f>
+        <v>5.8054840148050301E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1480,16 +1640,24 @@
         <f>F31</f>
         <v>5853</v>
       </c>
-      <c r="K26" s="11">
-        <f t="shared" si="1"/>
+      <c r="K26" s="12">
+        <f>J26/J21</f>
         <v>0.48766872187968674</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26">
         <f>K26*L21</f>
-        <v>9224.7752909043047</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+        <v>8095.1715067025634</v>
+      </c>
+      <c r="M26">
+        <f>J26/J16</f>
+        <v>4.0030366449177235E-2</v>
+      </c>
+      <c r="N26">
+        <f>J26/J6</f>
+        <v>9.2247752909043051E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1515,16 +1683,24 @@
         <f>F5</f>
         <v>505537</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="12">
         <f>J27/J12</f>
         <v>5.0501587411949607E-2</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27">
         <f>K27*L12</f>
         <v>20375.642929429781</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <f>J27/J12</f>
+        <v>5.0501587411949607E-2</v>
+      </c>
+      <c r="N27">
+        <f>J27/J2</f>
+        <v>2.0375642929429783E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1550,16 +1726,24 @@
         <f>F11</f>
         <v>69675</v>
       </c>
-      <c r="K28" s="11">
+      <c r="K28" s="12">
         <f>J28/J13</f>
         <v>5.2969524372823346E-2</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28">
         <f>K28*L13</f>
         <v>11376.269860305774</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <f>J28/J13</f>
+        <v>5.2969524372823346E-2</v>
+      </c>
+      <c r="N28">
+        <f>J28/J3</f>
+        <v>1.1376269860305774E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1585,16 +1769,24 @@
         <f>F17</f>
         <v>77780</v>
       </c>
-      <c r="K29" s="11">
+      <c r="K29" s="12">
         <f>J29/J14</f>
         <v>5.4352307492344695E-2</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L29">
         <f>K29*L14</f>
         <v>8777.4238069282728</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <f>J29/J14</f>
+        <v>5.4352307492344695E-2</v>
+      </c>
+      <c r="N29">
+        <f>J29/J4</f>
+        <v>8.7774238069282737E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1620,16 +1812,24 @@
         <f>F23</f>
         <v>56846</v>
       </c>
-      <c r="K30" s="11">
+      <c r="K30" s="12">
         <f>J30/J15</f>
         <v>2.7099849831954806E-2</v>
       </c>
-      <c r="L30" s="12">
+      <c r="L30">
         <f>K30*L15</f>
         <v>16753.06078001963</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="M30">
+        <f>J30/J15</f>
+        <v>2.7099849831954806E-2</v>
+      </c>
+      <c r="N30">
+        <f>J30/J5</f>
+        <v>1.6753060780019632E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -1655,16 +1855,24 @@
         <f>F29</f>
         <v>6936</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K31" s="12">
         <f>J31/J16</f>
         <v>4.7437317903894292E-2</v>
       </c>
-      <c r="L31" s="12">
+      <c r="L31">
         <f>K31*L16</f>
-        <v>10931.666054623656</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+        <v>9593.0479361846883</v>
+      </c>
+      <c r="M31">
+        <f>J31/J16</f>
+        <v>4.7437317903894292E-2</v>
+      </c>
+      <c r="N31">
+        <f>J31/J6</f>
+        <v>1.0931666054623656E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="I32" s="3" t="s">
         <v>37</v>
       </c>
@@ -1672,9 +1880,8 @@
         <f>SUM(J22,J27)</f>
         <v>1081294</v>
       </c>
-      <c r="K32" s="11"/>
-    </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I33" s="3" t="s">
         <v>38</v>
       </c>
@@ -1682,9 +1889,8 @@
         <f>SUM(J23,J28)</f>
         <v>112958</v>
       </c>
-      <c r="K33" s="11"/>
-    </row>
-    <row r="34" spans="9:11" ht="30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="9:10" ht="30" x14ac:dyDescent="0.2">
       <c r="I34" s="3" t="s">
         <v>39</v>
       </c>
@@ -1692,9 +1898,8 @@
         <f>SUM(J24,J29)</f>
         <v>134393</v>
       </c>
-      <c r="K34" s="11"/>
-    </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I35" s="3" t="s">
         <v>40</v>
       </c>
@@ -1702,9 +1907,8 @@
         <f>SUM(J25,J30)</f>
         <v>76545</v>
       </c>
-      <c r="K35" s="11"/>
-    </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I36" s="3" t="s">
         <v>41</v>
       </c>
@@ -1712,9 +1916,8 @@
         <f>SUM(J26,J31)</f>
         <v>12789</v>
       </c>
-      <c r="K36" s="11"/>
-    </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I37" s="3" t="s">
         <v>36</v>
       </c>
@@ -1722,9 +1925,8 @@
         <f>SUM(J32:J36)</f>
         <v>1417979</v>
       </c>
-      <c r="K37" s="11"/>
-    </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I38" s="3" t="s">
         <v>46</v>
       </c>
@@ -1732,9 +1934,8 @@
         <f>J37-J32</f>
         <v>336685</v>
       </c>
-      <c r="K38" s="11"/>
-    </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I39" s="3" t="s">
         <v>42</v>
       </c>
@@ -1742,9 +1943,8 @@
         <f>J37-J33</f>
         <v>1305021</v>
       </c>
-      <c r="K39" s="11"/>
-    </row>
-    <row r="40" spans="9:11" ht="30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="9:10" ht="30" x14ac:dyDescent="0.2">
       <c r="I40" s="3" t="s">
         <v>43</v>
       </c>
@@ -1752,9 +1952,8 @@
         <f>J37-J34</f>
         <v>1283586</v>
       </c>
-      <c r="K40" s="11"/>
-    </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I41" s="3" t="s">
         <v>44</v>
       </c>
@@ -1762,9 +1961,8 @@
         <f>J37-J35</f>
         <v>1341434</v>
       </c>
-      <c r="K41" s="11"/>
-    </row>
-    <row r="42" spans="9:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I42" s="3" t="s">
         <v>45</v>
       </c>
@@ -1772,7 +1970,6 @@
         <f>J37-J36</f>
         <v>1405190</v>
       </c>
-      <c r="K42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added in new data
</commit_message>
<xml_diff>
--- a/data/sankey_data.xlsx
+++ b/data/sankey_data.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25940" yWindow="9300" windowWidth="22160" windowHeight="17060"/>
+    <workbookView xWindow="1320" yWindow="2600" windowWidth="22160" windowHeight="17060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sankey data" sheetId="1" r:id="rId1"/>
+    <sheet name="REVISED" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
   <si>
     <t>wbhao</t>
   </si>
@@ -201,6 +202,18 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>all_number</t>
+  </si>
+  <si>
+    <t>all_percent</t>
+  </si>
+  <si>
+    <t>bachelor_number</t>
+  </si>
+  <si>
+    <t>bachelor_percent</t>
   </si>
 </sst>
 </file>
@@ -210,7 +223,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -233,12 +246,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -254,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -270,8 +289,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -589,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -849,7 +871,7 @@
         <v>23408059</v>
       </c>
       <c r="K7" s="12">
-        <f>J7/J2</f>
+        <f t="shared" ref="K7:K15" si="0">J7/J2</f>
         <v>0.94346062079536253</v>
       </c>
       <c r="L7">
@@ -888,7 +910,7 @@
         <v>5453028</v>
       </c>
       <c r="K8" s="12">
-        <f>J8/J3</f>
+        <f t="shared" si="0"/>
         <v>0.8903497392723857</v>
       </c>
       <c r="L8" s="2">
@@ -927,11 +949,11 @@
         <v>6659753</v>
       </c>
       <c r="K9" s="12">
-        <f>J9/J4</f>
+        <f t="shared" si="0"/>
         <v>0.7515489139941115</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L9" si="0">K9*L4</f>
+        <f t="shared" ref="L9" si="1">K9*L4</f>
         <v>751548.91399411147</v>
       </c>
       <c r="N9">
@@ -966,11 +988,11 @@
         <v>3227421</v>
       </c>
       <c r="K10" s="12">
-        <f>J10/J5</f>
+        <f t="shared" si="0"/>
         <v>0.95115188712858856</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" ref="L10" si="1">K10*L4</f>
+        <f t="shared" ref="L10" si="2">K10*L4</f>
         <v>951151.88712858851</v>
       </c>
       <c r="N10">
@@ -1005,11 +1027,11 @@
         <v>556792</v>
       </c>
       <c r="K11" s="12">
-        <f>J11/J6</f>
+        <f t="shared" si="0"/>
         <v>0.8775467424864497</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11" si="2">K11*L6</f>
+        <f t="shared" ref="L11" si="3">K11*L6</f>
         <v>877546.74248644966</v>
       </c>
       <c r="N11">
@@ -1044,11 +1066,11 @@
         <v>10010319</v>
       </c>
       <c r="K12" s="12">
-        <f>J12/J7</f>
+        <f t="shared" si="0"/>
         <v>0.42764412888740583</v>
       </c>
       <c r="L12">
-        <f>K12*L7</f>
+        <f t="shared" ref="L12:L26" si="4">K12*L7</f>
         <v>403465.39531960391</v>
       </c>
       <c r="M12">
@@ -1086,11 +1108,11 @@
         <v>1315379</v>
       </c>
       <c r="K13" s="12">
-        <f>J13/J8</f>
+        <f t="shared" si="0"/>
         <v>0.24121992404953724</v>
       </c>
       <c r="L13">
-        <f>K13*L8</f>
+        <f t="shared" si="4"/>
         <v>214770.09648481017</v>
       </c>
       <c r="M13">
@@ -1128,11 +1150,11 @@
         <v>1431034</v>
       </c>
       <c r="K14" s="12">
-        <f>J14/J9</f>
+        <f t="shared" si="0"/>
         <v>0.21487793916681294</v>
       </c>
       <c r="L14">
-        <f>K14*L9</f>
+        <f t="shared" si="4"/>
         <v>161491.28182211102</v>
       </c>
       <c r="M14">
@@ -1170,11 +1192,11 @@
         <v>2097650</v>
       </c>
       <c r="K15" s="12">
-        <f>J15/J10</f>
+        <f t="shared" si="0"/>
         <v>0.64994619542972543</v>
       </c>
       <c r="L15">
-        <f>K15*L10</f>
+        <f t="shared" si="4"/>
         <v>618197.55031502969</v>
       </c>
       <c r="M15">
@@ -1216,7 +1238,7 @@
         <v>0.23044443778989956</v>
       </c>
       <c r="L16">
-        <f>K16*L11</f>
+        <f t="shared" si="4"/>
         <v>202225.76570664765</v>
       </c>
       <c r="M16">
@@ -1254,11 +1276,11 @@
         <v>913874</v>
       </c>
       <c r="K17" s="12">
-        <f>J17/J12</f>
+        <f t="shared" ref="K17:K26" si="5">J17/J12</f>
         <v>9.1293194552541229E-2</v>
       </c>
       <c r="L17">
-        <f>K17*L12</f>
+        <f t="shared" si="4"/>
         <v>36833.644830130557</v>
       </c>
       <c r="M17">
@@ -1297,11 +1319,11 @@
         <v>83039</v>
       </c>
       <c r="K18" s="12">
-        <f>J18/J13</f>
+        <f t="shared" si="5"/>
         <v>6.312933382698066E-2</v>
       </c>
       <c r="L18">
-        <f>K18*L13</f>
+        <f t="shared" si="4"/>
         <v>13558.293117042427</v>
       </c>
       <c r="M18">
@@ -1340,11 +1362,11 @@
         <v>101986</v>
       </c>
       <c r="K19" s="12">
-        <f>J19/J14</f>
+        <f t="shared" si="5"/>
         <v>7.1267349343202183E-2</v>
       </c>
       <c r="L19">
-        <f>K19*L14</f>
+        <f t="shared" si="4"/>
         <v>11509.055597497902</v>
       </c>
       <c r="M19">
@@ -1383,11 +1405,11 @@
         <v>52831</v>
       </c>
       <c r="K20" s="12">
-        <f>J20/J15</f>
+        <f t="shared" si="5"/>
         <v>2.5185803160679809E-2</v>
       </c>
       <c r="L20">
-        <f>K20*L15</f>
+        <f t="shared" si="4"/>
         <v>15569.801816648791</v>
       </c>
       <c r="M20">
@@ -1426,11 +1448,11 @@
         <v>12002</v>
       </c>
       <c r="K21" s="12">
-        <f>J21/J16</f>
+        <f t="shared" si="5"/>
         <v>8.2085162843503354E-2</v>
       </c>
       <c r="L21">
-        <f>K21*L16</f>
+        <f t="shared" si="4"/>
         <v>16599.734909182327</v>
       </c>
       <c r="M21">
@@ -1469,11 +1491,11 @@
         <v>575757</v>
       </c>
       <c r="K22" s="12">
-        <f>J22/J17</f>
+        <f t="shared" si="5"/>
         <v>0.63001792369626453</v>
       </c>
       <c r="L22">
-        <f>K22*L17</f>
+        <f t="shared" si="4"/>
         <v>23205.856438044502</v>
       </c>
       <c r="M22">
@@ -1512,11 +1534,11 @@
         <v>43283</v>
       </c>
       <c r="K23" s="12">
-        <f>J23/J18</f>
+        <f t="shared" si="5"/>
         <v>0.52123700911619841</v>
       </c>
       <c r="L23">
-        <f>K23*L18</f>
+        <f t="shared" si="4"/>
         <v>7067.0841530479338</v>
       </c>
       <c r="M23">
@@ -1555,11 +1577,11 @@
         <v>56613</v>
       </c>
       <c r="K24" s="12">
-        <f>J24/J19</f>
+        <f t="shared" si="5"/>
         <v>0.55510560272978648</v>
       </c>
       <c r="L24">
-        <f>K24*L19</f>
+        <f t="shared" si="4"/>
         <v>6388.7412442996956</v>
       </c>
       <c r="M24">
@@ -1598,11 +1620,11 @@
         <v>19699</v>
       </c>
       <c r="K25" s="12">
-        <f>J25/J20</f>
+        <f t="shared" si="5"/>
         <v>0.37286820238117774</v>
       </c>
       <c r="L25">
-        <f>K25*L20</f>
+        <f t="shared" si="4"/>
         <v>5805.4840148050298</v>
       </c>
       <c r="M25">
@@ -1641,11 +1663,11 @@
         <v>5853</v>
       </c>
       <c r="K26" s="12">
-        <f>J26/J21</f>
+        <f t="shared" si="5"/>
         <v>0.48766872187968674</v>
       </c>
       <c r="L26">
-        <f>K26*L21</f>
+        <f t="shared" si="4"/>
         <v>8095.1715067025634</v>
       </c>
       <c r="M26">
@@ -1969,6 +1991,866 @@
       <c r="J42" s="2">
         <f>J37-J36</f>
         <v>1405190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="12"/>
+    <col min="10" max="10" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>5719544</v>
+      </c>
+      <c r="G2">
+        <f>SUM(F2:F7)</f>
+        <v>98058434</v>
+      </c>
+      <c r="H2" s="12">
+        <v>1</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>53694780</v>
+      </c>
+      <c r="G3">
+        <f>SUM(F3:F7)</f>
+        <v>92338890</v>
+      </c>
+      <c r="H3" s="12">
+        <f>G3/G2</f>
+        <v>0.94167208503452138</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>32876708</v>
+      </c>
+      <c r="G4">
+        <f>SUM(F4:F7)</f>
+        <v>38644110</v>
+      </c>
+      <c r="H4" s="12">
+        <f>G4/G2</f>
+        <v>0.39409266927513853</v>
+      </c>
+      <c r="I4">
+        <f>SUM(F4:F7)</f>
+        <v>38644110</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1970062</v>
+      </c>
+      <c r="G5">
+        <f>F5</f>
+        <v>1970062</v>
+      </c>
+      <c r="H5" s="12">
+        <f>G5/G2</f>
+        <v>2.0090694085528635E-2</v>
+      </c>
+      <c r="I5">
+        <f>F5</f>
+        <v>1970062</v>
+      </c>
+      <c r="J5" s="12">
+        <f>I5/I4</f>
+        <v>5.0979618886293411E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1377959</v>
+      </c>
+      <c r="G6">
+        <f>SUM(F6:F7)</f>
+        <v>3797340</v>
+      </c>
+      <c r="H6" s="12">
+        <f>G6/G2</f>
+        <v>3.8725276807908229E-2</v>
+      </c>
+      <c r="I6">
+        <f>SUM(F6:F7)</f>
+        <v>3797340</v>
+      </c>
+      <c r="J6" s="12">
+        <f>I6/I4</f>
+        <v>9.8264392684939569E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2419381</v>
+      </c>
+      <c r="G7">
+        <f>F7</f>
+        <v>2419381</v>
+      </c>
+      <c r="H7" s="12">
+        <f>G7/G2</f>
+        <v>2.4672849660234222E-2</v>
+      </c>
+      <c r="I7">
+        <f>F7</f>
+        <v>2419381</v>
+      </c>
+      <c r="J7" s="12">
+        <f>I7/I4</f>
+        <v>6.2606720661958576E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2680402</v>
+      </c>
+      <c r="G8">
+        <f>SUM(F8:F13)</f>
+        <v>22240873</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>15047057</v>
+      </c>
+      <c r="G9">
+        <f>SUM(F9:F13)</f>
+        <v>19560471</v>
+      </c>
+      <c r="H9" s="12">
+        <f>G9/G8</f>
+        <v>0.87948305806161475</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>3964872</v>
+      </c>
+      <c r="G10">
+        <f>SUM(F10:F13)</f>
+        <v>4513414</v>
+      </c>
+      <c r="H10" s="12">
+        <f>G10/G8</f>
+        <v>0.20293331111598004</v>
+      </c>
+      <c r="I10">
+        <f>SUM(F10:F13)</f>
+        <v>4513414</v>
+      </c>
+      <c r="J10" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>247003</v>
+      </c>
+      <c r="G11">
+        <f>F11</f>
+        <v>247003</v>
+      </c>
+      <c r="H11" s="12">
+        <f>G11/G8</f>
+        <v>1.1105814056849296E-2</v>
+      </c>
+      <c r="I11">
+        <f>F11</f>
+        <v>247003</v>
+      </c>
+      <c r="J11" s="12">
+        <f>I11/I10</f>
+        <v>5.472642217177507E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>144573</v>
+      </c>
+      <c r="G12">
+        <f>SUM(F12:F13)</f>
+        <v>301539</v>
+      </c>
+      <c r="H12" s="12">
+        <f>G12/G8</f>
+        <v>1.3557876077975897E-2</v>
+      </c>
+      <c r="I12">
+        <f>SUM(F12:F13)</f>
+        <v>301539</v>
+      </c>
+      <c r="J12" s="12">
+        <f>I12/I10</f>
+        <v>6.6809514925951843E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>156966</v>
+      </c>
+      <c r="G13">
+        <f>F13</f>
+        <v>156966</v>
+      </c>
+      <c r="H13" s="12">
+        <f>G13/G8</f>
+        <v>7.0575467069120892E-3</v>
+      </c>
+      <c r="I13">
+        <f>F13</f>
+        <v>156966</v>
+      </c>
+      <c r="J13" s="12">
+        <f>I13/I10</f>
+        <v>3.4777664978218263E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>9450292</v>
+      </c>
+      <c r="G14">
+        <f>SUM(F14:F19)</f>
+        <v>34884432</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>20190158</v>
+      </c>
+      <c r="G15">
+        <f>SUM(F15:F19)</f>
+        <v>25434140</v>
+      </c>
+      <c r="H15" s="12">
+        <f>G15/G14</f>
+        <v>0.72909715141699882</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>4535033</v>
+      </c>
+      <c r="G16">
+        <f>SUM(F16:F19)</f>
+        <v>5243982</v>
+      </c>
+      <c r="H16" s="12">
+        <f>G16/G14</f>
+        <v>0.15032441978702707</v>
+      </c>
+      <c r="I16">
+        <f>SUM(F16:F19)</f>
+        <v>5243982</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>312676</v>
+      </c>
+      <c r="G17">
+        <f>F17</f>
+        <v>312676</v>
+      </c>
+      <c r="H17" s="12">
+        <f>G17/G14</f>
+        <v>8.9631959608802002E-3</v>
+      </c>
+      <c r="I17">
+        <f>F17</f>
+        <v>312676</v>
+      </c>
+      <c r="J17" s="12">
+        <f>I17/I16</f>
+        <v>5.9625681400126848E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>181776</v>
+      </c>
+      <c r="G18">
+        <f>SUM(F18:F19)</f>
+        <v>396273</v>
+      </c>
+      <c r="H18" s="12">
+        <f>G18/G14</f>
+        <v>1.1359594446026812E-2</v>
+      </c>
+      <c r="I18">
+        <f>SUM(F18:F19)</f>
+        <v>396273</v>
+      </c>
+      <c r="J18" s="12">
+        <f>I18/I16</f>
+        <v>7.5567193022401682E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>214497</v>
+      </c>
+      <c r="G19">
+        <f>F19</f>
+        <v>214497</v>
+      </c>
+      <c r="H19" s="12">
+        <f>G19/G14</f>
+        <v>6.1487886630918918E-3</v>
+      </c>
+      <c r="I19">
+        <f>F19</f>
+        <v>214497</v>
+      </c>
+      <c r="J19" s="12">
+        <f>I19/I16</f>
+        <v>4.0903458478690431E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>578848</v>
+      </c>
+      <c r="G20">
+        <f>SUM(F20:F25)</f>
+        <v>10962316</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1</v>
+      </c>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>3393163</v>
+      </c>
+      <c r="G21">
+        <f>SUM(F21:F25)</f>
+        <v>10383468</v>
+      </c>
+      <c r="H21" s="12">
+        <f>G21/G20</f>
+        <v>0.94719655955912962</v>
+      </c>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>6650814</v>
+      </c>
+      <c r="G22">
+        <f>SUM(F22:F25)</f>
+        <v>6990305</v>
+      </c>
+      <c r="H22" s="12">
+        <f>G22/G20</f>
+        <v>0.63766680325580838</v>
+      </c>
+      <c r="I22">
+        <f>SUM(F22:F25)</f>
+        <v>6990305</v>
+      </c>
+      <c r="J22" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>168835</v>
+      </c>
+      <c r="G23">
+        <f>F23</f>
+        <v>168835</v>
+      </c>
+      <c r="H23" s="12">
+        <f>G23/G20</f>
+        <v>1.540139875551845E-2</v>
+      </c>
+      <c r="I23">
+        <f>F23</f>
+        <v>168835</v>
+      </c>
+      <c r="J23" s="12">
+        <f>I23/I22</f>
+        <v>2.4152737255384422E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>112934</v>
+      </c>
+      <c r="G24">
+        <f>SUM(F24:F25)</f>
+        <v>170656</v>
+      </c>
+      <c r="H24" s="12">
+        <f>G24/G20</f>
+        <v>1.5567513288250403E-2</v>
+      </c>
+      <c r="I24">
+        <f>SUM(F24:F25)</f>
+        <v>170656</v>
+      </c>
+      <c r="J24" s="12">
+        <f>I24/I22</f>
+        <v>2.4413240910089045E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>57722</v>
+      </c>
+      <c r="G25">
+        <f>F25</f>
+        <v>57722</v>
+      </c>
+      <c r="H25" s="12">
+        <f>G25/G20</f>
+        <v>5.2654931676846392E-3</v>
+      </c>
+      <c r="I25">
+        <f>F25</f>
+        <v>57722</v>
+      </c>
+      <c r="J25" s="12">
+        <f>I25/I22</f>
+        <v>8.2574365496212252E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>